<commit_message>
update TitleX wizard info plus new docs worksheet
</commit_message>
<xml_diff>
--- a/SSM-websites-and-software.xlsx
+++ b/SSM-websites-and-software.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="38400" windowHeight="22720" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-32920" yWindow="440" windowWidth="32060" windowHeight="22140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DataProcSeqAndProcesses" sheetId="3" r:id="rId1"/>
     <sheet name="SSMWebsites" sheetId="1" r:id="rId2"/>
     <sheet name="ToDo" sheetId="2" r:id="rId3"/>
+    <sheet name="Documents" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="120">
   <si>
     <t>URL</t>
   </si>
@@ -359,9 +360,6 @@
     <t>**The "Finish" button has been hidden in an effort to improve the user experience. Problem: Now, any post-wizard user changes to the map are not preserved.</t>
   </si>
   <si>
-    <t>Wizard prototype (maintained for backwards compatibility) for caregivers supporting a child with special health needs and/or developmental disabilities requiring responses to these demographic questions: 1) state; 2) county; 3) race; 4) hispanic? 5) language; 6) child's age; 7) insurance; 8) health conditions. Text entry response dropdown lists tuned for CYSHCN caregiver audience. Identical to ssm-wizard-d/?module=CaregiversOfCYSHCN from the user's viewpoint. Decommissioned 2017/06/13.</t>
-  </si>
-  <si>
     <t>Green fill means that presence or absence of drop-down lists in this version corresponds to text (no mention of drop-down lists if there aren't any).</t>
   </si>
   <si>
@@ -375,13 +373,88 @@
   </si>
   <si>
     <t>CYSHCN: fixed 2017/06/13</t>
+  </si>
+  <si>
+    <t>Demographic questions?</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>state; county/municipality; race;  Hispanic?; language;  child's age; insurance; health conditions</t>
+  </si>
+  <si>
+    <t>position; grade[s]; age range; years at school;  race/ethnicity; school location</t>
+  </si>
+  <si>
+    <t>Wizard prototype (maintained for backwards compatibility). Identical to ssm-wizard-d/?module=CaregiversOfCYSHCN from the user's viewpoint. Decommissioned 2017/06/13: url redirects to http://syssci.renci.org/ssm-wizard-d/?module=CaregiversOfCYSHCN.</t>
+  </si>
+  <si>
+    <t>NA (decommissioned)</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm/blob/master/SSM-websites-and-software.xlsx</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm/blob/master/SSM_Processing_Sequence.txt</t>
+  </si>
+  <si>
+    <t>This spreadsheet</t>
+  </si>
+  <si>
+    <t>Text-only example runthrough : SSMs -&gt; BLMS -&gt; sort -&gt; CBLM -&gt; CM and CPN</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/sort/blob/master/Editing_Sorted_SSM_Documents.docx</t>
+  </si>
+  <si>
+    <t>Tips for manually editing sorted text items while maximizing the likelihood of the results being processable.</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/sort/blob/master/File_Formats_for_the_Sort_Segment_of_the_System_Support_Mapping_Processing_Sequence.docx</t>
+  </si>
+  <si>
+    <t>Details of the various sort file formats with emphasis on .json.</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/binary-link-matrix/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/sort/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/text2JSON/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/AddCodesToBLM/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/create_code_matrices/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>Also the README.md files in the various SSM-related GitHub repos:</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/extractMaps/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/get_mental_maps/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/add_codes_to_SSMs/blob/master/README.md</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -456,6 +529,21 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -501,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -534,6 +622,15 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -572,7 +669,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -699,38 +796,57 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="30" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="30" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="32">
@@ -769,14 +885,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1360,11 +1468,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K216"/>
+  <dimension ref="A1:L216"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1374,17 +1482,17 @@
     <col min="3" max="3" width="78.33203125" style="7" customWidth="1"/>
     <col min="4" max="4" width="38" style="21" customWidth="1"/>
     <col min="5" max="5" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27" style="8" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="18.5" style="5" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="31.1640625" style="5" customWidth="1"/>
-    <col min="12" max="15" width="27.6640625" style="5" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="5"/>
+    <col min="6" max="7" width="27" style="8" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="5" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="31.1640625" style="5" customWidth="1"/>
+    <col min="13" max="16" width="27.6640625" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="16" customHeight="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="16" customHeight="1">
       <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1394,10 +1502,11 @@
       <c r="D1" s="22"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="2"/>
+      <c r="H1" s="4"/>
       <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="120">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="120">
       <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
@@ -1417,16 +1526,19 @@
         <v>14</v>
       </c>
       <c r="G2" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60">
+    <row r="3" spans="1:12" ht="60">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -1445,17 +1557,20 @@
       <c r="F3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="140">
+    <row r="4" spans="1:12" ht="140">
       <c r="A4" s="13">
         <f>A3+1</f>
         <v>2</v>
@@ -1475,28 +1590,31 @@
       <c r="F4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="J4" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="48" t="s">
+      <c r="K4" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K4" s="49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="40">
+    </row>
+    <row r="5" spans="1:12" ht="40">
       <c r="A5" s="13">
         <f t="shared" ref="A5:A12" si="0">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="44" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -1509,22 +1627,25 @@
       <c r="F5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="I5" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="J5" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="60">
+    <row r="6" spans="1:12" ht="60">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="44" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -1537,56 +1658,62 @@
       <c r="F6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="I6" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="J6" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="158" customHeight="1">
-      <c r="A7" s="50">
+    <row r="7" spans="1:12" ht="90" customHeight="1">
+      <c r="A7" s="48">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="53" t="s">
+      <c r="C7" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="54" t="s">
+      <c r="E7" s="48"/>
+      <c r="F7" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="47" t="s">
+      <c r="G7" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="I7" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="J7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="K7" s="45" t="s">
+      <c r="K7" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="L7" s="55" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="100">
+    <row r="8" spans="1:12" ht="120">
       <c r="A8" s="13">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="44" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -1601,22 +1728,27 @@
       <c r="F8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="H8" s="17" t="s">
+      <c r="G8" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="J8" s="18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="100">
+      <c r="K8" s="54"/>
+      <c r="L8" s="56"/>
+    </row>
+    <row r="9" spans="1:12" ht="100">
       <c r="A9" s="13">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="44" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -1631,22 +1763,25 @@
       <c r="F9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="47" t="s">
+      <c r="G9" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="I9" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="J9" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="84" customHeight="1">
+    <row r="10" spans="1:12" ht="84" customHeight="1">
       <c r="A10" s="13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -1664,19 +1799,22 @@
       <c r="G10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="I10" s="14" t="s">
+      <c r="H10" s="16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="120">
+      <c r="I10" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="120">
       <c r="A11" s="13">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="44" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -1689,22 +1827,25 @@
       <c r="F11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="47" t="s">
+      <c r="G11" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="J11" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="80">
+    <row r="12" spans="1:12" ht="80">
       <c r="A12" s="13">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1719,605 +1860,814 @@
       <c r="F12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="47" t="s">
+      <c r="G12" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="J12" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="6:6">
+    <row r="22" spans="6:7">
       <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="6:6">
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="6:7">
       <c r="F23" s="21"/>
-    </row>
-    <row r="24" spans="6:6">
+      <c r="G23" s="21"/>
+    </row>
+    <row r="24" spans="6:7">
       <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="6:6">
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="6:7">
       <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="6:6">
+      <c r="G25" s="21"/>
+    </row>
+    <row r="26" spans="6:7">
       <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="6:6">
+      <c r="G26" s="21"/>
+    </row>
+    <row r="27" spans="6:7">
       <c r="F27" s="21"/>
-    </row>
-    <row r="28" spans="6:6">
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="6:7">
       <c r="F28" s="21"/>
-    </row>
-    <row r="29" spans="6:6">
+      <c r="G28" s="21"/>
+    </row>
+    <row r="29" spans="6:7">
       <c r="F29" s="21"/>
-    </row>
-    <row r="30" spans="6:6">
+      <c r="G29" s="21"/>
+    </row>
+    <row r="30" spans="6:7">
       <c r="F30" s="21"/>
-    </row>
-    <row r="31" spans="6:6">
+      <c r="G30" s="21"/>
+    </row>
+    <row r="31" spans="6:7">
       <c r="F31" s="21"/>
-    </row>
-    <row r="32" spans="6:6">
+      <c r="G31" s="21"/>
+    </row>
+    <row r="32" spans="6:7">
       <c r="F32" s="21"/>
-    </row>
-    <row r="33" spans="6:6">
+      <c r="G32" s="21"/>
+    </row>
+    <row r="33" spans="6:7">
       <c r="F33" s="21"/>
-    </row>
-    <row r="34" spans="6:6">
+      <c r="G33" s="21"/>
+    </row>
+    <row r="34" spans="6:7">
       <c r="F34" s="21"/>
-    </row>
-    <row r="35" spans="6:6">
+      <c r="G34" s="21"/>
+    </row>
+    <row r="35" spans="6:7">
       <c r="F35" s="21"/>
-    </row>
-    <row r="36" spans="6:6">
+      <c r="G35" s="21"/>
+    </row>
+    <row r="36" spans="6:7">
       <c r="F36" s="21"/>
-    </row>
-    <row r="37" spans="6:6">
+      <c r="G36" s="21"/>
+    </row>
+    <row r="37" spans="6:7">
       <c r="F37" s="21"/>
-    </row>
-    <row r="38" spans="6:6">
+      <c r="G37" s="21"/>
+    </row>
+    <row r="38" spans="6:7">
       <c r="F38" s="21"/>
-    </row>
-    <row r="39" spans="6:6">
+      <c r="G38" s="21"/>
+    </row>
+    <row r="39" spans="6:7">
       <c r="F39" s="21"/>
-    </row>
-    <row r="40" spans="6:6">
+      <c r="G39" s="21"/>
+    </row>
+    <row r="40" spans="6:7">
       <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="6:6">
+      <c r="G40" s="21"/>
+    </row>
+    <row r="41" spans="6:7">
       <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="6:6">
+      <c r="G41" s="21"/>
+    </row>
+    <row r="42" spans="6:7">
       <c r="F42" s="21"/>
-    </row>
-    <row r="43" spans="6:6">
+      <c r="G42" s="21"/>
+    </row>
+    <row r="43" spans="6:7">
       <c r="F43" s="21"/>
-    </row>
-    <row r="44" spans="6:6">
+      <c r="G43" s="21"/>
+    </row>
+    <row r="44" spans="6:7">
       <c r="F44" s="21"/>
-    </row>
-    <row r="45" spans="6:6">
+      <c r="G44" s="21"/>
+    </row>
+    <row r="45" spans="6:7">
       <c r="F45" s="21"/>
-    </row>
-    <row r="46" spans="6:6">
+      <c r="G45" s="21"/>
+    </row>
+    <row r="46" spans="6:7">
       <c r="F46" s="21"/>
-    </row>
-    <row r="47" spans="6:6">
+      <c r="G46" s="21"/>
+    </row>
+    <row r="47" spans="6:7">
       <c r="F47" s="21"/>
-    </row>
-    <row r="48" spans="6:6">
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="6:7">
       <c r="F48" s="21"/>
-    </row>
-    <row r="49" spans="6:6">
+      <c r="G48" s="21"/>
+    </row>
+    <row r="49" spans="6:7">
       <c r="F49" s="21"/>
-    </row>
-    <row r="50" spans="6:6">
+      <c r="G49" s="21"/>
+    </row>
+    <row r="50" spans="6:7">
       <c r="F50" s="21"/>
-    </row>
-    <row r="51" spans="6:6">
+      <c r="G50" s="21"/>
+    </row>
+    <row r="51" spans="6:7">
       <c r="F51" s="21"/>
-    </row>
-    <row r="52" spans="6:6">
+      <c r="G51" s="21"/>
+    </row>
+    <row r="52" spans="6:7">
       <c r="F52" s="21"/>
-    </row>
-    <row r="53" spans="6:6">
+      <c r="G52" s="21"/>
+    </row>
+    <row r="53" spans="6:7">
       <c r="F53" s="21"/>
-    </row>
-    <row r="54" spans="6:6">
+      <c r="G53" s="21"/>
+    </row>
+    <row r="54" spans="6:7">
       <c r="F54" s="21"/>
-    </row>
-    <row r="55" spans="6:6">
+      <c r="G54" s="21"/>
+    </row>
+    <row r="55" spans="6:7">
       <c r="F55" s="21"/>
-    </row>
-    <row r="56" spans="6:6">
+      <c r="G55" s="21"/>
+    </row>
+    <row r="56" spans="6:7">
       <c r="F56" s="21"/>
-    </row>
-    <row r="57" spans="6:6">
+      <c r="G56" s="21"/>
+    </row>
+    <row r="57" spans="6:7">
       <c r="F57" s="21"/>
-    </row>
-    <row r="58" spans="6:6">
+      <c r="G57" s="21"/>
+    </row>
+    <row r="58" spans="6:7">
       <c r="F58" s="21"/>
-    </row>
-    <row r="59" spans="6:6">
+      <c r="G58" s="21"/>
+    </row>
+    <row r="59" spans="6:7">
       <c r="F59" s="21"/>
-    </row>
-    <row r="60" spans="6:6">
+      <c r="G59" s="21"/>
+    </row>
+    <row r="60" spans="6:7">
       <c r="F60" s="21"/>
-    </row>
-    <row r="61" spans="6:6">
+      <c r="G60" s="21"/>
+    </row>
+    <row r="61" spans="6:7">
       <c r="F61" s="21"/>
-    </row>
-    <row r="62" spans="6:6">
+      <c r="G61" s="21"/>
+    </row>
+    <row r="62" spans="6:7">
       <c r="F62" s="21"/>
-    </row>
-    <row r="63" spans="6:6">
+      <c r="G62" s="21"/>
+    </row>
+    <row r="63" spans="6:7">
       <c r="F63" s="21"/>
-    </row>
-    <row r="64" spans="6:6">
+      <c r="G63" s="21"/>
+    </row>
+    <row r="64" spans="6:7">
       <c r="F64" s="21"/>
-    </row>
-    <row r="65" spans="6:6">
+      <c r="G64" s="21"/>
+    </row>
+    <row r="65" spans="6:7">
       <c r="F65" s="21"/>
-    </row>
-    <row r="66" spans="6:6">
+      <c r="G65" s="21"/>
+    </row>
+    <row r="66" spans="6:7">
       <c r="F66" s="21"/>
-    </row>
-    <row r="67" spans="6:6">
+      <c r="G66" s="21"/>
+    </row>
+    <row r="67" spans="6:7">
       <c r="F67" s="21"/>
-    </row>
-    <row r="68" spans="6:6">
+      <c r="G67" s="21"/>
+    </row>
+    <row r="68" spans="6:7">
       <c r="F68" s="21"/>
-    </row>
-    <row r="69" spans="6:6">
+      <c r="G68" s="21"/>
+    </row>
+    <row r="69" spans="6:7">
       <c r="F69" s="21"/>
-    </row>
-    <row r="70" spans="6:6">
+      <c r="G69" s="21"/>
+    </row>
+    <row r="70" spans="6:7">
       <c r="F70" s="21"/>
-    </row>
-    <row r="71" spans="6:6">
+      <c r="G70" s="21"/>
+    </row>
+    <row r="71" spans="6:7">
       <c r="F71" s="21"/>
-    </row>
-    <row r="72" spans="6:6">
+      <c r="G71" s="21"/>
+    </row>
+    <row r="72" spans="6:7">
       <c r="F72" s="21"/>
-    </row>
-    <row r="73" spans="6:6">
+      <c r="G72" s="21"/>
+    </row>
+    <row r="73" spans="6:7">
       <c r="F73" s="21"/>
-    </row>
-    <row r="74" spans="6:6">
+      <c r="G73" s="21"/>
+    </row>
+    <row r="74" spans="6:7">
       <c r="F74" s="21"/>
-    </row>
-    <row r="75" spans="6:6">
+      <c r="G74" s="21"/>
+    </row>
+    <row r="75" spans="6:7">
       <c r="F75" s="21"/>
-    </row>
-    <row r="76" spans="6:6">
+      <c r="G75" s="21"/>
+    </row>
+    <row r="76" spans="6:7">
       <c r="F76" s="21"/>
-    </row>
-    <row r="77" spans="6:6">
+      <c r="G76" s="21"/>
+    </row>
+    <row r="77" spans="6:7">
       <c r="F77" s="21"/>
-    </row>
-    <row r="78" spans="6:6">
+      <c r="G77" s="21"/>
+    </row>
+    <row r="78" spans="6:7">
       <c r="F78" s="21"/>
-    </row>
-    <row r="79" spans="6:6">
+      <c r="G78" s="21"/>
+    </row>
+    <row r="79" spans="6:7">
       <c r="F79" s="21"/>
-    </row>
-    <row r="80" spans="6:6">
+      <c r="G79" s="21"/>
+    </row>
+    <row r="80" spans="6:7">
       <c r="F80" s="21"/>
-    </row>
-    <row r="81" spans="6:6">
+      <c r="G80" s="21"/>
+    </row>
+    <row r="81" spans="6:7">
       <c r="F81" s="21"/>
-    </row>
-    <row r="82" spans="6:6">
+      <c r="G81" s="21"/>
+    </row>
+    <row r="82" spans="6:7">
       <c r="F82" s="21"/>
-    </row>
-    <row r="83" spans="6:6">
+      <c r="G82" s="21"/>
+    </row>
+    <row r="83" spans="6:7">
       <c r="F83" s="21"/>
-    </row>
-    <row r="84" spans="6:6">
+      <c r="G83" s="21"/>
+    </row>
+    <row r="84" spans="6:7">
       <c r="F84" s="21"/>
-    </row>
-    <row r="85" spans="6:6">
+      <c r="G84" s="21"/>
+    </row>
+    <row r="85" spans="6:7">
       <c r="F85" s="21"/>
-    </row>
-    <row r="86" spans="6:6">
+      <c r="G85" s="21"/>
+    </row>
+    <row r="86" spans="6:7">
       <c r="F86" s="21"/>
-    </row>
-    <row r="87" spans="6:6">
+      <c r="G86" s="21"/>
+    </row>
+    <row r="87" spans="6:7">
       <c r="F87" s="21"/>
-    </row>
-    <row r="88" spans="6:6">
+      <c r="G87" s="21"/>
+    </row>
+    <row r="88" spans="6:7">
       <c r="F88" s="21"/>
-    </row>
-    <row r="89" spans="6:6">
+      <c r="G88" s="21"/>
+    </row>
+    <row r="89" spans="6:7">
       <c r="F89" s="21"/>
-    </row>
-    <row r="90" spans="6:6">
+      <c r="G89" s="21"/>
+    </row>
+    <row r="90" spans="6:7">
       <c r="F90" s="21"/>
-    </row>
-    <row r="91" spans="6:6">
+      <c r="G90" s="21"/>
+    </row>
+    <row r="91" spans="6:7">
       <c r="F91" s="21"/>
-    </row>
-    <row r="92" spans="6:6">
+      <c r="G91" s="21"/>
+    </row>
+    <row r="92" spans="6:7">
       <c r="F92" s="21"/>
-    </row>
-    <row r="93" spans="6:6">
+      <c r="G92" s="21"/>
+    </row>
+    <row r="93" spans="6:7">
       <c r="F93" s="21"/>
-    </row>
-    <row r="94" spans="6:6">
+      <c r="G93" s="21"/>
+    </row>
+    <row r="94" spans="6:7">
       <c r="F94" s="21"/>
-    </row>
-    <row r="95" spans="6:6">
+      <c r="G94" s="21"/>
+    </row>
+    <row r="95" spans="6:7">
       <c r="F95" s="21"/>
-    </row>
-    <row r="96" spans="6:6">
+      <c r="G95" s="21"/>
+    </row>
+    <row r="96" spans="6:7">
       <c r="F96" s="21"/>
-    </row>
-    <row r="97" spans="6:6">
+      <c r="G96" s="21"/>
+    </row>
+    <row r="97" spans="6:7">
       <c r="F97" s="21"/>
-    </row>
-    <row r="98" spans="6:6">
+      <c r="G97" s="21"/>
+    </row>
+    <row r="98" spans="6:7">
       <c r="F98" s="21"/>
-    </row>
-    <row r="99" spans="6:6">
+      <c r="G98" s="21"/>
+    </row>
+    <row r="99" spans="6:7">
       <c r="F99" s="21"/>
-    </row>
-    <row r="100" spans="6:6">
+      <c r="G99" s="21"/>
+    </row>
+    <row r="100" spans="6:7">
       <c r="F100" s="21"/>
-    </row>
-    <row r="101" spans="6:6">
+      <c r="G100" s="21"/>
+    </row>
+    <row r="101" spans="6:7">
       <c r="F101" s="21"/>
-    </row>
-    <row r="102" spans="6:6">
+      <c r="G101" s="21"/>
+    </row>
+    <row r="102" spans="6:7">
       <c r="F102" s="21"/>
-    </row>
-    <row r="103" spans="6:6">
+      <c r="G102" s="21"/>
+    </row>
+    <row r="103" spans="6:7">
       <c r="F103" s="21"/>
-    </row>
-    <row r="104" spans="6:6">
+      <c r="G103" s="21"/>
+    </row>
+    <row r="104" spans="6:7">
       <c r="F104" s="21"/>
-    </row>
-    <row r="105" spans="6:6">
+      <c r="G104" s="21"/>
+    </row>
+    <row r="105" spans="6:7">
       <c r="F105" s="21"/>
-    </row>
-    <row r="106" spans="6:6">
+      <c r="G105" s="21"/>
+    </row>
+    <row r="106" spans="6:7">
       <c r="F106" s="21"/>
-    </row>
-    <row r="107" spans="6:6">
+      <c r="G106" s="21"/>
+    </row>
+    <row r="107" spans="6:7">
       <c r="F107" s="21"/>
-    </row>
-    <row r="108" spans="6:6">
+      <c r="G107" s="21"/>
+    </row>
+    <row r="108" spans="6:7">
       <c r="F108" s="21"/>
-    </row>
-    <row r="109" spans="6:6">
+      <c r="G108" s="21"/>
+    </row>
+    <row r="109" spans="6:7">
       <c r="F109" s="21"/>
-    </row>
-    <row r="110" spans="6:6">
+      <c r="G109" s="21"/>
+    </row>
+    <row r="110" spans="6:7">
       <c r="F110" s="21"/>
-    </row>
-    <row r="111" spans="6:6">
+      <c r="G110" s="21"/>
+    </row>
+    <row r="111" spans="6:7">
       <c r="F111" s="21"/>
-    </row>
-    <row r="112" spans="6:6">
+      <c r="G111" s="21"/>
+    </row>
+    <row r="112" spans="6:7">
       <c r="F112" s="21"/>
-    </row>
-    <row r="113" spans="6:6">
+      <c r="G112" s="21"/>
+    </row>
+    <row r="113" spans="6:7">
       <c r="F113" s="21"/>
-    </row>
-    <row r="114" spans="6:6">
+      <c r="G113" s="21"/>
+    </row>
+    <row r="114" spans="6:7">
       <c r="F114" s="21"/>
-    </row>
-    <row r="115" spans="6:6">
+      <c r="G114" s="21"/>
+    </row>
+    <row r="115" spans="6:7">
       <c r="F115" s="21"/>
-    </row>
-    <row r="116" spans="6:6">
+      <c r="G115" s="21"/>
+    </row>
+    <row r="116" spans="6:7">
       <c r="F116" s="21"/>
-    </row>
-    <row r="117" spans="6:6">
+      <c r="G116" s="21"/>
+    </row>
+    <row r="117" spans="6:7">
       <c r="F117" s="21"/>
-    </row>
-    <row r="118" spans="6:6">
+      <c r="G117" s="21"/>
+    </row>
+    <row r="118" spans="6:7">
       <c r="F118" s="21"/>
-    </row>
-    <row r="119" spans="6:6">
+      <c r="G118" s="21"/>
+    </row>
+    <row r="119" spans="6:7">
       <c r="F119" s="21"/>
-    </row>
-    <row r="120" spans="6:6">
+      <c r="G119" s="21"/>
+    </row>
+    <row r="120" spans="6:7">
       <c r="F120" s="21"/>
-    </row>
-    <row r="121" spans="6:6">
+      <c r="G120" s="21"/>
+    </row>
+    <row r="121" spans="6:7">
       <c r="F121" s="21"/>
-    </row>
-    <row r="122" spans="6:6">
+      <c r="G121" s="21"/>
+    </row>
+    <row r="122" spans="6:7">
       <c r="F122" s="21"/>
-    </row>
-    <row r="123" spans="6:6">
+      <c r="G122" s="21"/>
+    </row>
+    <row r="123" spans="6:7">
       <c r="F123" s="21"/>
-    </row>
-    <row r="124" spans="6:6">
+      <c r="G123" s="21"/>
+    </row>
+    <row r="124" spans="6:7">
       <c r="F124" s="21"/>
-    </row>
-    <row r="125" spans="6:6">
+      <c r="G124" s="21"/>
+    </row>
+    <row r="125" spans="6:7">
       <c r="F125" s="21"/>
-    </row>
-    <row r="126" spans="6:6">
+      <c r="G125" s="21"/>
+    </row>
+    <row r="126" spans="6:7">
       <c r="F126" s="21"/>
-    </row>
-    <row r="127" spans="6:6">
+      <c r="G126" s="21"/>
+    </row>
+    <row r="127" spans="6:7">
       <c r="F127" s="21"/>
-    </row>
-    <row r="128" spans="6:6">
+      <c r="G127" s="21"/>
+    </row>
+    <row r="128" spans="6:7">
       <c r="F128" s="21"/>
-    </row>
-    <row r="129" spans="6:6">
+      <c r="G128" s="21"/>
+    </row>
+    <row r="129" spans="6:7">
       <c r="F129" s="21"/>
-    </row>
-    <row r="130" spans="6:6">
+      <c r="G129" s="21"/>
+    </row>
+    <row r="130" spans="6:7">
       <c r="F130" s="21"/>
-    </row>
-    <row r="131" spans="6:6">
+      <c r="G130" s="21"/>
+    </row>
+    <row r="131" spans="6:7">
       <c r="F131" s="21"/>
-    </row>
-    <row r="132" spans="6:6">
+      <c r="G131" s="21"/>
+    </row>
+    <row r="132" spans="6:7">
       <c r="F132" s="21"/>
-    </row>
-    <row r="133" spans="6:6">
+      <c r="G132" s="21"/>
+    </row>
+    <row r="133" spans="6:7">
       <c r="F133" s="21"/>
-    </row>
-    <row r="134" spans="6:6">
+      <c r="G133" s="21"/>
+    </row>
+    <row r="134" spans="6:7">
       <c r="F134" s="21"/>
-    </row>
-    <row r="135" spans="6:6">
+      <c r="G134" s="21"/>
+    </row>
+    <row r="135" spans="6:7">
       <c r="F135" s="21"/>
-    </row>
-    <row r="136" spans="6:6">
+      <c r="G135" s="21"/>
+    </row>
+    <row r="136" spans="6:7">
       <c r="F136" s="21"/>
-    </row>
-    <row r="137" spans="6:6">
+      <c r="G136" s="21"/>
+    </row>
+    <row r="137" spans="6:7">
       <c r="F137" s="21"/>
-    </row>
-    <row r="138" spans="6:6">
+      <c r="G137" s="21"/>
+    </row>
+    <row r="138" spans="6:7">
       <c r="F138" s="21"/>
-    </row>
-    <row r="139" spans="6:6">
+      <c r="G138" s="21"/>
+    </row>
+    <row r="139" spans="6:7">
       <c r="F139" s="21"/>
-    </row>
-    <row r="140" spans="6:6">
+      <c r="G139" s="21"/>
+    </row>
+    <row r="140" spans="6:7">
       <c r="F140" s="21"/>
-    </row>
-    <row r="141" spans="6:6">
+      <c r="G140" s="21"/>
+    </row>
+    <row r="141" spans="6:7">
       <c r="F141" s="21"/>
-    </row>
-    <row r="142" spans="6:6">
+      <c r="G141" s="21"/>
+    </row>
+    <row r="142" spans="6:7">
       <c r="F142" s="21"/>
-    </row>
-    <row r="143" spans="6:6">
+      <c r="G142" s="21"/>
+    </row>
+    <row r="143" spans="6:7">
       <c r="F143" s="21"/>
-    </row>
-    <row r="144" spans="6:6">
+      <c r="G143" s="21"/>
+    </row>
+    <row r="144" spans="6:7">
       <c r="F144" s="21"/>
-    </row>
-    <row r="145" spans="6:6">
+      <c r="G144" s="21"/>
+    </row>
+    <row r="145" spans="6:7">
       <c r="F145" s="21"/>
-    </row>
-    <row r="146" spans="6:6">
+      <c r="G145" s="21"/>
+    </row>
+    <row r="146" spans="6:7">
       <c r="F146" s="21"/>
-    </row>
-    <row r="147" spans="6:6">
+      <c r="G146" s="21"/>
+    </row>
+    <row r="147" spans="6:7">
       <c r="F147" s="21"/>
-    </row>
-    <row r="148" spans="6:6">
+      <c r="G147" s="21"/>
+    </row>
+    <row r="148" spans="6:7">
       <c r="F148" s="21"/>
-    </row>
-    <row r="149" spans="6:6">
+      <c r="G148" s="21"/>
+    </row>
+    <row r="149" spans="6:7">
       <c r="F149" s="21"/>
-    </row>
-    <row r="150" spans="6:6">
+      <c r="G149" s="21"/>
+    </row>
+    <row r="150" spans="6:7">
       <c r="F150" s="21"/>
-    </row>
-    <row r="151" spans="6:6">
+      <c r="G150" s="21"/>
+    </row>
+    <row r="151" spans="6:7">
       <c r="F151" s="21"/>
-    </row>
-    <row r="152" spans="6:6">
+      <c r="G151" s="21"/>
+    </row>
+    <row r="152" spans="6:7">
       <c r="F152" s="21"/>
-    </row>
-    <row r="153" spans="6:6">
+      <c r="G152" s="21"/>
+    </row>
+    <row r="153" spans="6:7">
       <c r="F153" s="21"/>
-    </row>
-    <row r="154" spans="6:6">
+      <c r="G153" s="21"/>
+    </row>
+    <row r="154" spans="6:7">
       <c r="F154" s="21"/>
-    </row>
-    <row r="155" spans="6:6">
+      <c r="G154" s="21"/>
+    </row>
+    <row r="155" spans="6:7">
       <c r="F155" s="21"/>
-    </row>
-    <row r="156" spans="6:6">
+      <c r="G155" s="21"/>
+    </row>
+    <row r="156" spans="6:7">
       <c r="F156" s="21"/>
-    </row>
-    <row r="157" spans="6:6">
+      <c r="G156" s="21"/>
+    </row>
+    <row r="157" spans="6:7">
       <c r="F157" s="21"/>
-    </row>
-    <row r="158" spans="6:6">
+      <c r="G157" s="21"/>
+    </row>
+    <row r="158" spans="6:7">
       <c r="F158" s="21"/>
-    </row>
-    <row r="159" spans="6:6">
+      <c r="G158" s="21"/>
+    </row>
+    <row r="159" spans="6:7">
       <c r="F159" s="21"/>
-    </row>
-    <row r="160" spans="6:6">
+      <c r="G159" s="21"/>
+    </row>
+    <row r="160" spans="6:7">
       <c r="F160" s="21"/>
-    </row>
-    <row r="161" spans="6:6">
+      <c r="G160" s="21"/>
+    </row>
+    <row r="161" spans="6:7">
       <c r="F161" s="21"/>
-    </row>
-    <row r="162" spans="6:6">
+      <c r="G161" s="21"/>
+    </row>
+    <row r="162" spans="6:7">
       <c r="F162" s="21"/>
-    </row>
-    <row r="163" spans="6:6">
+      <c r="G162" s="21"/>
+    </row>
+    <row r="163" spans="6:7">
       <c r="F163" s="21"/>
-    </row>
-    <row r="164" spans="6:6">
+      <c r="G163" s="21"/>
+    </row>
+    <row r="164" spans="6:7">
       <c r="F164" s="21"/>
-    </row>
-    <row r="165" spans="6:6">
+      <c r="G164" s="21"/>
+    </row>
+    <row r="165" spans="6:7">
       <c r="F165" s="21"/>
-    </row>
-    <row r="166" spans="6:6">
+      <c r="G165" s="21"/>
+    </row>
+    <row r="166" spans="6:7">
       <c r="F166" s="21"/>
-    </row>
-    <row r="167" spans="6:6">
+      <c r="G166" s="21"/>
+    </row>
+    <row r="167" spans="6:7">
       <c r="F167" s="21"/>
-    </row>
-    <row r="168" spans="6:6">
+      <c r="G167" s="21"/>
+    </row>
+    <row r="168" spans="6:7">
       <c r="F168" s="21"/>
-    </row>
-    <row r="169" spans="6:6">
+      <c r="G168" s="21"/>
+    </row>
+    <row r="169" spans="6:7">
       <c r="F169" s="21"/>
-    </row>
-    <row r="170" spans="6:6">
+      <c r="G169" s="21"/>
+    </row>
+    <row r="170" spans="6:7">
       <c r="F170" s="21"/>
-    </row>
-    <row r="171" spans="6:6">
+      <c r="G170" s="21"/>
+    </row>
+    <row r="171" spans="6:7">
       <c r="F171" s="21"/>
-    </row>
-    <row r="172" spans="6:6">
+      <c r="G171" s="21"/>
+    </row>
+    <row r="172" spans="6:7">
       <c r="F172" s="21"/>
-    </row>
-    <row r="173" spans="6:6">
+      <c r="G172" s="21"/>
+    </row>
+    <row r="173" spans="6:7">
       <c r="F173" s="21"/>
-    </row>
-    <row r="174" spans="6:6">
+      <c r="G173" s="21"/>
+    </row>
+    <row r="174" spans="6:7">
       <c r="F174" s="21"/>
-    </row>
-    <row r="175" spans="6:6">
+      <c r="G174" s="21"/>
+    </row>
+    <row r="175" spans="6:7">
       <c r="F175" s="21"/>
-    </row>
-    <row r="176" spans="6:6">
+      <c r="G175" s="21"/>
+    </row>
+    <row r="176" spans="6:7">
       <c r="F176" s="21"/>
-    </row>
-    <row r="177" spans="6:6">
+      <c r="G176" s="21"/>
+    </row>
+    <row r="177" spans="6:7">
       <c r="F177" s="21"/>
-    </row>
-    <row r="178" spans="6:6">
+      <c r="G177" s="21"/>
+    </row>
+    <row r="178" spans="6:7">
       <c r="F178" s="21"/>
-    </row>
-    <row r="179" spans="6:6">
+      <c r="G178" s="21"/>
+    </row>
+    <row r="179" spans="6:7">
       <c r="F179" s="21"/>
-    </row>
-    <row r="180" spans="6:6">
+      <c r="G179" s="21"/>
+    </row>
+    <row r="180" spans="6:7">
       <c r="F180" s="21"/>
-    </row>
-    <row r="181" spans="6:6">
+      <c r="G180" s="21"/>
+    </row>
+    <row r="181" spans="6:7">
       <c r="F181" s="21"/>
-    </row>
-    <row r="182" spans="6:6">
+      <c r="G181" s="21"/>
+    </row>
+    <row r="182" spans="6:7">
       <c r="F182" s="21"/>
-    </row>
-    <row r="183" spans="6:6">
+      <c r="G182" s="21"/>
+    </row>
+    <row r="183" spans="6:7">
       <c r="F183" s="21"/>
-    </row>
-    <row r="184" spans="6:6">
+      <c r="G183" s="21"/>
+    </row>
+    <row r="184" spans="6:7">
       <c r="F184" s="21"/>
-    </row>
-    <row r="185" spans="6:6">
+      <c r="G184" s="21"/>
+    </row>
+    <row r="185" spans="6:7">
       <c r="F185" s="21"/>
-    </row>
-    <row r="186" spans="6:6">
+      <c r="G185" s="21"/>
+    </row>
+    <row r="186" spans="6:7">
       <c r="F186" s="21"/>
-    </row>
-    <row r="187" spans="6:6">
+      <c r="G186" s="21"/>
+    </row>
+    <row r="187" spans="6:7">
       <c r="F187" s="21"/>
-    </row>
-    <row r="188" spans="6:6">
+      <c r="G187" s="21"/>
+    </row>
+    <row r="188" spans="6:7">
       <c r="F188" s="21"/>
-    </row>
-    <row r="189" spans="6:6">
+      <c r="G188" s="21"/>
+    </row>
+    <row r="189" spans="6:7">
       <c r="F189" s="21"/>
-    </row>
-    <row r="190" spans="6:6">
+      <c r="G189" s="21"/>
+    </row>
+    <row r="190" spans="6:7">
       <c r="F190" s="21"/>
-    </row>
-    <row r="191" spans="6:6">
+      <c r="G190" s="21"/>
+    </row>
+    <row r="191" spans="6:7">
       <c r="F191" s="21"/>
-    </row>
-    <row r="192" spans="6:6">
+      <c r="G191" s="21"/>
+    </row>
+    <row r="192" spans="6:7">
       <c r="F192" s="21"/>
-    </row>
-    <row r="193" spans="6:6">
+      <c r="G192" s="21"/>
+    </row>
+    <row r="193" spans="6:7">
       <c r="F193" s="21"/>
-    </row>
-    <row r="194" spans="6:6">
+      <c r="G193" s="21"/>
+    </row>
+    <row r="194" spans="6:7">
       <c r="F194" s="21"/>
-    </row>
-    <row r="195" spans="6:6">
+      <c r="G194" s="21"/>
+    </row>
+    <row r="195" spans="6:7">
       <c r="F195" s="21"/>
-    </row>
-    <row r="196" spans="6:6">
+      <c r="G195" s="21"/>
+    </row>
+    <row r="196" spans="6:7">
       <c r="F196" s="21"/>
-    </row>
-    <row r="197" spans="6:6">
+      <c r="G196" s="21"/>
+    </row>
+    <row r="197" spans="6:7">
       <c r="F197" s="21"/>
-    </row>
-    <row r="198" spans="6:6">
+      <c r="G197" s="21"/>
+    </row>
+    <row r="198" spans="6:7">
       <c r="F198" s="21"/>
-    </row>
-    <row r="199" spans="6:6">
+      <c r="G198" s="21"/>
+    </row>
+    <row r="199" spans="6:7">
       <c r="F199" s="21"/>
-    </row>
-    <row r="200" spans="6:6">
+      <c r="G199" s="21"/>
+    </row>
+    <row r="200" spans="6:7">
       <c r="F200" s="21"/>
-    </row>
-    <row r="201" spans="6:6">
+      <c r="G200" s="21"/>
+    </row>
+    <row r="201" spans="6:7">
       <c r="F201" s="21"/>
-    </row>
-    <row r="202" spans="6:6">
+      <c r="G201" s="21"/>
+    </row>
+    <row r="202" spans="6:7">
       <c r="F202" s="21"/>
-    </row>
-    <row r="203" spans="6:6">
+      <c r="G202" s="21"/>
+    </row>
+    <row r="203" spans="6:7">
       <c r="F203" s="21"/>
-    </row>
-    <row r="204" spans="6:6">
+      <c r="G203" s="21"/>
+    </row>
+    <row r="204" spans="6:7">
       <c r="F204" s="21"/>
-    </row>
-    <row r="205" spans="6:6">
+      <c r="G204" s="21"/>
+    </row>
+    <row r="205" spans="6:7">
       <c r="F205" s="21"/>
-    </row>
-    <row r="206" spans="6:6">
+      <c r="G205" s="21"/>
+    </row>
+    <row r="206" spans="6:7">
       <c r="F206" s="21"/>
-    </row>
-    <row r="207" spans="6:6">
+      <c r="G206" s="21"/>
+    </row>
+    <row r="207" spans="6:7">
       <c r="F207" s="21"/>
-    </row>
-    <row r="208" spans="6:6">
+      <c r="G207" s="21"/>
+    </row>
+    <row r="208" spans="6:7">
       <c r="F208" s="21"/>
-    </row>
-    <row r="209" spans="6:6">
+      <c r="G208" s="21"/>
+    </row>
+    <row r="209" spans="6:7">
       <c r="F209" s="21"/>
-    </row>
-    <row r="210" spans="6:6">
+      <c r="G209" s="21"/>
+    </row>
+    <row r="210" spans="6:7">
       <c r="F210" s="21"/>
-    </row>
-    <row r="211" spans="6:6">
+      <c r="G210" s="21"/>
+    </row>
+    <row r="211" spans="6:7">
       <c r="F211" s="21"/>
-    </row>
-    <row r="212" spans="6:6">
+      <c r="G211" s="21"/>
+    </row>
+    <row r="212" spans="6:7">
       <c r="F212" s="21"/>
-    </row>
-    <row r="213" spans="6:6">
+      <c r="G212" s="21"/>
+    </row>
+    <row r="213" spans="6:7">
       <c r="F213" s="21"/>
-    </row>
-    <row r="214" spans="6:6">
+      <c r="G213" s="21"/>
+    </row>
+    <row r="214" spans="6:7">
       <c r="F214" s="21"/>
-    </row>
-    <row r="215" spans="6:6">
+      <c r="G214" s="21"/>
+    </row>
+    <row r="215" spans="6:7">
       <c r="F215" s="21"/>
-    </row>
-    <row r="216" spans="6:6">
+      <c r="G215" s="21"/>
+    </row>
+    <row r="216" spans="6:7">
       <c r="F216" s="21"/>
+      <c r="G216" s="21"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="B12" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup scale="35" fitToHeight="2" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2333,8 +2683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2410,4 +2760,123 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="76.33203125" style="60" customWidth="1"/>
+    <col min="2" max="2" width="104.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="58" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="57" customFormat="1">
+      <c r="A2" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30">
+      <c r="A6" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="61" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="60" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="60" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="60" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="60" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="60" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="60" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update to include new TitleV and TitleX wizards, plus additions to to-do list
</commit_message>
<xml_diff>
--- a/SSM-websites-and-software.xlsx
+++ b/SSM-websites-and-software.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-32920" yWindow="440" windowWidth="32060" windowHeight="22140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-34520" yWindow="880" windowWidth="32060" windowHeight="22140" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DataProcSeqAndProcesses" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="136">
   <si>
     <t>URL</t>
   </si>
@@ -54,13 +54,7 @@
     <t>http://syssci.renci.org/ssm-wizard-mental-health-in-schools/</t>
   </si>
   <si>
-    <t>http://syssci.renci.org/ssm-wizard-family-planning</t>
-  </si>
-  <si>
     <t>The SSM family of websites and related software</t>
-  </si>
-  <si>
-    <t>tbd</t>
   </si>
   <si>
     <t>http://syssci.renci.org/force-directed-map/</t>
@@ -232,12 +226,6 @@
     <t>Post-processing software</t>
   </si>
   <si>
-    <t>Dropdown lists for text entry</t>
-  </si>
-  <si>
-    <t>ssm-wizard for UNC-CH doctoral student Amber Dawn Haley's work on Family Planning project/Title X.  Based on http://syssci.renci.org/ssm-wizard/?module=TitleVWorkforce but includes custom text and demographic questions. No text entry response dropdown lists.</t>
-  </si>
-  <si>
     <t>Qualtrics survey link*</t>
   </si>
   <si>
@@ -257,9 +245,6 @@
   </si>
   <si>
     <t>Ensure reference to drop down lists is appropriate (matches the presence/absence of drop down lists)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Still in use? </t>
   </si>
   <si>
     <t>Y</t>
@@ -366,9 +351,6 @@
     <t>Gray fill means this website is decommissioned, i.e., the user can't see it and is instead redirected to another website.</t>
   </si>
   <si>
-    <t>planned</t>
-  </si>
-  <si>
     <t>* Should the Qualtrics surveys be removed? Who's using them? 2017/06/05: we're keeping them and adding one for TitleX/Family Planning.</t>
   </si>
   <si>
@@ -405,9 +387,6 @@
     <t>This spreadsheet</t>
   </si>
   <si>
-    <t>Text-only example runthrough : SSMs -&gt; BLMS -&gt; sort -&gt; CBLM -&gt; CM and CPN</t>
-  </si>
-  <si>
     <t>https://github.com/steve9000gi/sort/blob/master/Editing_Sorted_SSM_Documents.docx</t>
   </si>
   <si>
@@ -448,6 +427,75 @@
   </si>
   <si>
     <t>https://github.com/steve9000gi/add_codes_to_SSMs/blob/master/README.md</t>
+  </si>
+  <si>
+    <t>Text-only example runthrough : SSMs -&gt; BLMS -&gt; sort -&gt; CBLM -&gt; CM and CPM</t>
+  </si>
+  <si>
+    <t>8/10/2017 for all SSM Wizard versions:</t>
+  </si>
+  <si>
+    <t>Restore hidden ""Finish" button as "Save" (doesn't close wizard)</t>
+  </si>
+  <si>
+    <t>Fix Minimize</t>
+  </si>
+  <si>
+    <t>Enforce limits on zoom and translate</t>
+  </si>
+  <si>
+    <t>Fix completions (elements of completions objects should be arrays)</t>
+  </si>
+  <si>
+    <t>Add wizard type (e.g., TitleX or TitleV), version number, and timestamp to source and to SSM json output</t>
+  </si>
+  <si>
+    <t>http://syssci.renci.org/ssm-wizard-TitleX</t>
+  </si>
+  <si>
+    <t>First Name, Last Name, Title/Position, Agency/Organization Name, Agency/Organization Type, State, County or equivalent, City, reason for using the System Support Mapper</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>"Finish" converted to "Save"</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm/tree/wizard-TitleX</t>
+  </si>
+  <si>
+    <t>http://syssci.renci.org/ssm-wizard-TitleV</t>
+  </si>
+  <si>
+    <t>https://github.com/steve9000gi/ssm/tree/wizard-TitleV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In use? </t>
+  </si>
+  <si>
+    <t>Draft TitleX questions need to be updated</t>
+  </si>
+  <si>
+    <t>For "Role" only</t>
+  </si>
+  <si>
+    <t>ssm-wizard for Family Planning project/Title X. Based on http://syssci.renci.org/ssm-wizard/?module=TitleVWorkforce but includes custom text and demographic questions.Text entry response dropdown completions list for "Role" only.</t>
+  </si>
+  <si>
+    <t>ssm-wizard for Maternal and Child Health/Title V. Based on http://syssci.renci.org/ssm-wizard/?module=TitleVWorkforce but includes custom text and demographic questions. No text entry response dropdown completions lists.</t>
+  </si>
+  <si>
+    <t>Dropdown completions lists for text entry</t>
+  </si>
+  <si>
+    <t>ALL (done for ssm-wizard-TitleX and ssm-wizard-TitleV)</t>
+  </si>
+  <si>
+    <t>ALL (done for ssm-wizard-TitleX)</t>
+  </si>
+  <si>
+    <t>ALL (type only displayed for ssm-wizard-TitleX and ssm-wizard-TitleV)</t>
   </si>
 </sst>
 </file>
@@ -545,7 +593,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -585,6 +633,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3FFF8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,7 +689,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -668,8 +722,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -823,18 +879,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -848,8 +892,30 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="30" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="32">
+  <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -873,6 +939,8 @@
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
@@ -1272,10 +1340,10 @@
     <row r="2" spans="1:7" ht="178" customHeight="1"/>
     <row r="4" spans="1:7" s="28" customFormat="1" ht="24">
       <c r="A4" s="23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>1</v>
@@ -1284,10 +1352,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G4" s="27"/>
     </row>
@@ -1296,19 +1364,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="33" customFormat="1" ht="132">
@@ -1317,19 +1385,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" s="34"/>
     </row>
@@ -1339,19 +1407,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" s="30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G7" s="34"/>
     </row>
@@ -1361,19 +1429,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G8" s="34"/>
     </row>
@@ -1383,19 +1451,19 @@
         <v>5</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G9" s="34"/>
     </row>
@@ -1405,19 +1473,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G10" s="34"/>
     </row>
@@ -1427,19 +1495,19 @@
         <v>7</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" s="34"/>
     </row>
@@ -1468,11 +1536,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L216"/>
+  <dimension ref="A1:L217"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1494,7 +1562,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="16" customHeight="1">
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3">
         <v>42891</v>
@@ -1508,7 +1576,7 @@
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="120">
       <c r="A2" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>0</v>
@@ -1520,22 +1588,22 @@
         <v>2</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="60">
@@ -1546,28 +1614,28 @@
         <v>3</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H3" s="45" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="140">
@@ -1579,65 +1647,65 @@
         <v>4</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H4" s="45" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K4" s="46" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="L4" s="47" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="40">
       <c r="A5" s="13">
-        <f t="shared" ref="A5:A12" si="0">A4+1</f>
+        <f t="shared" ref="A5:A13" si="0">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="44" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="43" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="60">
@@ -1649,26 +1717,26 @@
         <v>6</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H6" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>66</v>
-      </c>
       <c r="J6" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="90" customHeight="1">
@@ -1680,32 +1748,34 @@
         <v>7</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="48"/>
+        <v>35</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>14</v>
+      </c>
       <c r="F7" s="51" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G7" s="51" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H7" s="45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="L7" s="55" t="s">
-        <v>89</v>
+        <v>13</v>
+      </c>
+      <c r="K7" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="L7" s="60" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="120">
@@ -1717,31 +1787,31 @@
         <v>8</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H8" s="45" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="54"/>
-      <c r="L8" s="56"/>
+        <v>13</v>
+      </c>
+      <c r="K8" s="59"/>
+      <c r="L8" s="61"/>
     </row>
     <row r="9" spans="1:12" ht="100">
       <c r="A9" s="13">
@@ -1752,130 +1822,159 @@
         <v>9</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H9" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="189" customHeight="1">
+      <c r="A10" s="13">
+        <f>A8+1</f>
+        <v>7</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="84" customHeight="1">
+      <c r="A11" s="13">
+        <f>A9+1</f>
+        <v>8</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="I9" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="84" customHeight="1">
-      <c r="A10" s="13">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="120">
-      <c r="A11" s="13">
+      <c r="J11" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="120">
+      <c r="A12" s="13">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B12" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="80">
-      <c r="A12" s="13">
+      <c r="F12" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="80">
+      <c r="A13" s="13">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="13" t="s">
+      <c r="B13" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="6:7">
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
+      <c r="C13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="23" spans="6:7">
       <c r="F23" s="21"/>
@@ -2652,6 +2751,10 @@
     <row r="216" spans="6:7">
       <c r="F216" s="21"/>
       <c r="G216" s="21"/>
+    </row>
+    <row r="217" spans="6:7">
+      <c r="F217" s="21"/>
+      <c r="G217" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2665,9 +2768,11 @@
     <hyperlink ref="B7" r:id="rId3"/>
     <hyperlink ref="B8" r:id="rId4"/>
     <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId6"/>
+    <hyperlink ref="B12" r:id="rId7"/>
+    <hyperlink ref="B13" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup scale="35" fitToHeight="2" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2681,10 +2786,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2697,40 +2802,40 @@
     <row r="1" spans="1:3" s="38" customFormat="1">
       <c r="A1" s="41"/>
       <c r="B1" s="39" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="42" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="42" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="42" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -2738,22 +2843,76 @@
     </row>
     <row r="5" spans="1:3" ht="45">
       <c r="A5" s="42" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="42" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>87</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="62" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="65" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2766,109 +2925,109 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="76.33203125" style="60" customWidth="1"/>
+    <col min="1" max="1" width="76.33203125" style="56" customWidth="1"/>
     <col min="2" max="2" width="104.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="53" customFormat="1">
+      <c r="A2" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30">
+      <c r="A6" s="56" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="57" customFormat="1">
-      <c r="A2" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="59" t="s">
+      <c r="B6" t="s">
         <v>102</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="56" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="56" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="60" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="56" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30">
-      <c r="A6" s="60" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="B6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="61" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="60" t="s">
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="56" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="60" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="56" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="60" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="56" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="60" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="60" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="60" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="60" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="60" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="60" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix version, add timestamp
</commit_message>
<xml_diff>
--- a/SSM-websites-and-software.xlsx
+++ b/SSM-websites-and-software.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-34520" yWindow="880" windowWidth="32060" windowHeight="22140" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-38400" yWindow="-440" windowWidth="38400" windowHeight="22720" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataProcSeqAndProcesses" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="137">
   <si>
     <t>URL</t>
   </si>
@@ -496,6 +496,9 @@
   </si>
   <si>
     <t>ALL (type only displayed for ssm-wizard-TitleX and ssm-wizard-TitleV)</t>
+  </si>
+  <si>
+    <t>Version/ Timestamp</t>
   </si>
 </sst>
 </file>
@@ -725,7 +728,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -751,18 +754,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -780,9 +771,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -914,6 +902,18 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -1329,195 +1329,195 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="37"/>
-    <col min="2" max="2" width="16.83203125" style="37" customWidth="1"/>
-    <col min="3" max="3" width="91.5" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="37" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="37"/>
+    <col min="1" max="1" width="8.83203125" style="32"/>
+    <col min="2" max="2" width="16.83203125" style="32" customWidth="1"/>
+    <col min="3" max="3" width="91.5" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="32" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="382" customHeight="1"/>
     <row r="2" spans="1:7" ht="178" customHeight="1"/>
-    <row r="4" spans="1:7" s="28" customFormat="1" ht="24">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:7" s="23" customFormat="1" ht="24">
+      <c r="A4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="27"/>
-    </row>
-    <row r="5" spans="1:7" s="33" customFormat="1" ht="170" customHeight="1">
-      <c r="A5" s="29">
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" s="28" customFormat="1" ht="170" customHeight="1">
+      <c r="A5" s="24">
         <v>1</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="33" customFormat="1" ht="132">
-      <c r="A6" s="29">
+    <row r="6" spans="1:7" s="28" customFormat="1" ht="132">
+      <c r="A6" s="24">
         <f t="shared" ref="A6:A11" si="0">A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="34"/>
-    </row>
-    <row r="7" spans="1:7" s="33" customFormat="1" ht="48">
-      <c r="A7" s="29">
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="1:7" s="28" customFormat="1" ht="48">
+      <c r="A7" s="24">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="34"/>
-    </row>
-    <row r="8" spans="1:7" s="33" customFormat="1" ht="96">
-      <c r="A8" s="29">
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:7" s="28" customFormat="1" ht="96">
+      <c r="A8" s="24">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="34"/>
-    </row>
-    <row r="9" spans="1:7" s="33" customFormat="1" ht="24">
-      <c r="A9" s="29">
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" spans="1:7" s="28" customFormat="1" ht="24">
+      <c r="A9" s="24">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="34"/>
-    </row>
-    <row r="10" spans="1:7" s="33" customFormat="1" ht="60">
-      <c r="A10" s="29">
+      <c r="G9" s="29"/>
+    </row>
+    <row r="10" spans="1:7" s="28" customFormat="1" ht="60">
+      <c r="A10" s="24">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="34"/>
-    </row>
-    <row r="11" spans="1:7" s="33" customFormat="1" ht="48">
-      <c r="A11" s="29">
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="1:7" s="28" customFormat="1" ht="48">
+      <c r="A11" s="24">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="34"/>
-    </row>
-    <row r="12" spans="1:7" s="33" customFormat="1">
-      <c r="B12" s="34"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="1:7" s="28" customFormat="1">
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1536,11 +1536,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L217"/>
+  <dimension ref="A1:M217"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1548,1218 +1548,1254 @@
     <col min="1" max="1" width="5" style="5" customWidth="1"/>
     <col min="2" max="2" width="56.83203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="78.33203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="38" style="21" customWidth="1"/>
+    <col min="4" max="4" width="38" style="16" customWidth="1"/>
     <col min="5" max="5" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="27" style="8" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" style="6" customWidth="1"/>
     <col min="9" max="9" width="14.83203125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="31.1640625" style="5" customWidth="1"/>
-    <col min="13" max="16" width="27.6640625" style="5" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="5"/>
+    <col min="10" max="10" width="14.33203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="18.5" style="5" customWidth="1"/>
+    <col min="12" max="12" width="27.6640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="31.1640625" style="5" customWidth="1"/>
+    <col min="14" max="17" width="27.6640625" style="5" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="16" customHeight="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="16" customHeight="1">
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="3">
         <v>42891</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="17"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="120">
-      <c r="A2" s="9" t="s">
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" s="64" customFormat="1" ht="120">
+      <c r="A2" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="61" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="62" t="s">
+        <v>136</v>
+      </c>
+      <c r="K2" s="62" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="60">
-      <c r="A3" s="13">
+    <row r="3" spans="1:13" ht="60">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="140">
-      <c r="A4" s="13">
+    <row r="4" spans="1:13" ht="140">
+      <c r="A4" s="9">
         <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="46" t="s">
+      <c r="L4" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="L4" s="47" t="s">
+      <c r="M4" s="42" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="40">
-      <c r="A5" s="13">
+    <row r="5" spans="1:13" ht="40">
+      <c r="A5" s="9">
         <f t="shared" ref="A5:A13" si="0">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="16" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="60">
-      <c r="A6" s="13">
+      <c r="K5" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="60">
+      <c r="A6" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="16" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="45" t="s">
+      <c r="H6" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="90" customHeight="1">
-      <c r="A7" s="48">
+      <c r="K6" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="90" customHeight="1">
+      <c r="A7" s="43">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="G7" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="13"/>
+      <c r="K7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="58" t="s">
+      <c r="L7" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="L7" s="60" t="s">
+      <c r="M7" s="55" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="120">
-      <c r="A8" s="13">
+    <row r="8" spans="1:13" ht="120">
+      <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H8" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="59"/>
-      <c r="L8" s="61"/>
-    </row>
-    <row r="9" spans="1:12" ht="100">
-      <c r="A9" s="13">
+      <c r="L8" s="54"/>
+      <c r="M8" s="56"/>
+    </row>
+    <row r="9" spans="1:13" ht="100">
+      <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="45" t="s">
+      <c r="H9" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="189" customHeight="1">
-      <c r="A10" s="13">
+      <c r="K9" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="189" customHeight="1">
+      <c r="A10" s="9">
         <f>A8+1</f>
         <v>7</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="H10" s="64" t="s">
+      <c r="H10" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="84" customHeight="1">
-      <c r="A11" s="13">
+    <row r="11" spans="1:13" ht="84" customHeight="1">
+      <c r="A11" s="9">
         <f>A9+1</f>
         <v>8</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="45" t="s">
+      <c r="H11" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="120">
-      <c r="A12" s="13">
+    <row r="12" spans="1:13" ht="120">
+      <c r="A12" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="13" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="45" t="s">
+      <c r="H12" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="80">
-      <c r="A13" s="13">
+      <c r="K12" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="80">
+      <c r="A13" s="9">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="45" t="s">
+      <c r="H13" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="10" t="s">
         <v>65</v>
       </c>
+      <c r="K13" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="23" spans="6:7">
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="6:7">
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
     </row>
     <row r="25" spans="6:7">
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="26" spans="6:7">
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="6:7">
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
     </row>
     <row r="28" spans="6:7">
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="6:7">
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
     </row>
     <row r="30" spans="6:7">
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
     </row>
     <row r="31" spans="6:7">
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
     </row>
     <row r="32" spans="6:7">
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
     </row>
     <row r="33" spans="6:7">
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
     </row>
     <row r="34" spans="6:7">
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
     </row>
     <row r="35" spans="6:7">
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
     </row>
     <row r="36" spans="6:7">
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
     </row>
     <row r="37" spans="6:7">
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
     </row>
     <row r="38" spans="6:7">
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
     </row>
     <row r="39" spans="6:7">
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
     </row>
     <row r="40" spans="6:7">
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
     </row>
     <row r="41" spans="6:7">
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
     </row>
     <row r="42" spans="6:7">
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="6:7">
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
     </row>
     <row r="44" spans="6:7">
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
     </row>
     <row r="45" spans="6:7">
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
     </row>
     <row r="46" spans="6:7">
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
     </row>
     <row r="47" spans="6:7">
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="6:7">
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
     </row>
     <row r="49" spans="6:7">
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
     </row>
     <row r="50" spans="6:7">
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
     </row>
     <row r="51" spans="6:7">
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
     </row>
     <row r="52" spans="6:7">
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
     </row>
     <row r="53" spans="6:7">
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
     </row>
     <row r="54" spans="6:7">
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
     </row>
     <row r="55" spans="6:7">
-      <c r="F55" s="21"/>
-      <c r="G55" s="21"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
     </row>
     <row r="56" spans="6:7">
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
     </row>
     <row r="57" spans="6:7">
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
     </row>
     <row r="58" spans="6:7">
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
     </row>
     <row r="59" spans="6:7">
-      <c r="F59" s="21"/>
-      <c r="G59" s="21"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
     </row>
     <row r="60" spans="6:7">
-      <c r="F60" s="21"/>
-      <c r="G60" s="21"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
     </row>
     <row r="61" spans="6:7">
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
     </row>
     <row r="62" spans="6:7">
-      <c r="F62" s="21"/>
-      <c r="G62" s="21"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
     </row>
     <row r="63" spans="6:7">
-      <c r="F63" s="21"/>
-      <c r="G63" s="21"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
     </row>
     <row r="64" spans="6:7">
-      <c r="F64" s="21"/>
-      <c r="G64" s="21"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
     </row>
     <row r="65" spans="6:7">
-      <c r="F65" s="21"/>
-      <c r="G65" s="21"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
     </row>
     <row r="66" spans="6:7">
-      <c r="F66" s="21"/>
-      <c r="G66" s="21"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
     </row>
     <row r="67" spans="6:7">
-      <c r="F67" s="21"/>
-      <c r="G67" s="21"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
     </row>
     <row r="68" spans="6:7">
-      <c r="F68" s="21"/>
-      <c r="G68" s="21"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
     </row>
     <row r="69" spans="6:7">
-      <c r="F69" s="21"/>
-      <c r="G69" s="21"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="16"/>
     </row>
     <row r="70" spans="6:7">
-      <c r="F70" s="21"/>
-      <c r="G70" s="21"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
     </row>
     <row r="71" spans="6:7">
-      <c r="F71" s="21"/>
-      <c r="G71" s="21"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
     </row>
     <row r="72" spans="6:7">
-      <c r="F72" s="21"/>
-      <c r="G72" s="21"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
     </row>
     <row r="73" spans="6:7">
-      <c r="F73" s="21"/>
-      <c r="G73" s="21"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
     </row>
     <row r="74" spans="6:7">
-      <c r="F74" s="21"/>
-      <c r="G74" s="21"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
     </row>
     <row r="75" spans="6:7">
-      <c r="F75" s="21"/>
-      <c r="G75" s="21"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="16"/>
     </row>
     <row r="76" spans="6:7">
-      <c r="F76" s="21"/>
-      <c r="G76" s="21"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
     </row>
     <row r="77" spans="6:7">
-      <c r="F77" s="21"/>
-      <c r="G77" s="21"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
     </row>
     <row r="78" spans="6:7">
-      <c r="F78" s="21"/>
-      <c r="G78" s="21"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="16"/>
     </row>
     <row r="79" spans="6:7">
-      <c r="F79" s="21"/>
-      <c r="G79" s="21"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="16"/>
     </row>
     <row r="80" spans="6:7">
-      <c r="F80" s="21"/>
-      <c r="G80" s="21"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="16"/>
     </row>
     <row r="81" spans="6:7">
-      <c r="F81" s="21"/>
-      <c r="G81" s="21"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="16"/>
     </row>
     <row r="82" spans="6:7">
-      <c r="F82" s="21"/>
-      <c r="G82" s="21"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="16"/>
     </row>
     <row r="83" spans="6:7">
-      <c r="F83" s="21"/>
-      <c r="G83" s="21"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="16"/>
     </row>
     <row r="84" spans="6:7">
-      <c r="F84" s="21"/>
-      <c r="G84" s="21"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="16"/>
     </row>
     <row r="85" spans="6:7">
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
+      <c r="F85" s="16"/>
+      <c r="G85" s="16"/>
     </row>
     <row r="86" spans="6:7">
-      <c r="F86" s="21"/>
-      <c r="G86" s="21"/>
+      <c r="F86" s="16"/>
+      <c r="G86" s="16"/>
     </row>
     <row r="87" spans="6:7">
-      <c r="F87" s="21"/>
-      <c r="G87" s="21"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="16"/>
     </row>
     <row r="88" spans="6:7">
-      <c r="F88" s="21"/>
-      <c r="G88" s="21"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="16"/>
     </row>
     <row r="89" spans="6:7">
-      <c r="F89" s="21"/>
-      <c r="G89" s="21"/>
+      <c r="F89" s="16"/>
+      <c r="G89" s="16"/>
     </row>
     <row r="90" spans="6:7">
-      <c r="F90" s="21"/>
-      <c r="G90" s="21"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="16"/>
     </row>
     <row r="91" spans="6:7">
-      <c r="F91" s="21"/>
-      <c r="G91" s="21"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="16"/>
     </row>
     <row r="92" spans="6:7">
-      <c r="F92" s="21"/>
-      <c r="G92" s="21"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="16"/>
     </row>
     <row r="93" spans="6:7">
-      <c r="F93" s="21"/>
-      <c r="G93" s="21"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="16"/>
     </row>
     <row r="94" spans="6:7">
-      <c r="F94" s="21"/>
-      <c r="G94" s="21"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="16"/>
     </row>
     <row r="95" spans="6:7">
-      <c r="F95" s="21"/>
-      <c r="G95" s="21"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="16"/>
     </row>
     <row r="96" spans="6:7">
-      <c r="F96" s="21"/>
-      <c r="G96" s="21"/>
+      <c r="F96" s="16"/>
+      <c r="G96" s="16"/>
     </row>
     <row r="97" spans="6:7">
-      <c r="F97" s="21"/>
-      <c r="G97" s="21"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="16"/>
     </row>
     <row r="98" spans="6:7">
-      <c r="F98" s="21"/>
-      <c r="G98" s="21"/>
+      <c r="F98" s="16"/>
+      <c r="G98" s="16"/>
     </row>
     <row r="99" spans="6:7">
-      <c r="F99" s="21"/>
-      <c r="G99" s="21"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="16"/>
     </row>
     <row r="100" spans="6:7">
-      <c r="F100" s="21"/>
-      <c r="G100" s="21"/>
+      <c r="F100" s="16"/>
+      <c r="G100" s="16"/>
     </row>
     <row r="101" spans="6:7">
-      <c r="F101" s="21"/>
-      <c r="G101" s="21"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="16"/>
     </row>
     <row r="102" spans="6:7">
-      <c r="F102" s="21"/>
-      <c r="G102" s="21"/>
+      <c r="F102" s="16"/>
+      <c r="G102" s="16"/>
     </row>
     <row r="103" spans="6:7">
-      <c r="F103" s="21"/>
-      <c r="G103" s="21"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="16"/>
     </row>
     <row r="104" spans="6:7">
-      <c r="F104" s="21"/>
-      <c r="G104" s="21"/>
+      <c r="F104" s="16"/>
+      <c r="G104" s="16"/>
     </row>
     <row r="105" spans="6:7">
-      <c r="F105" s="21"/>
-      <c r="G105" s="21"/>
+      <c r="F105" s="16"/>
+      <c r="G105" s="16"/>
     </row>
     <row r="106" spans="6:7">
-      <c r="F106" s="21"/>
-      <c r="G106" s="21"/>
+      <c r="F106" s="16"/>
+      <c r="G106" s="16"/>
     </row>
     <row r="107" spans="6:7">
-      <c r="F107" s="21"/>
-      <c r="G107" s="21"/>
+      <c r="F107" s="16"/>
+      <c r="G107" s="16"/>
     </row>
     <row r="108" spans="6:7">
-      <c r="F108" s="21"/>
-      <c r="G108" s="21"/>
+      <c r="F108" s="16"/>
+      <c r="G108" s="16"/>
     </row>
     <row r="109" spans="6:7">
-      <c r="F109" s="21"/>
-      <c r="G109" s="21"/>
+      <c r="F109" s="16"/>
+      <c r="G109" s="16"/>
     </row>
     <row r="110" spans="6:7">
-      <c r="F110" s="21"/>
-      <c r="G110" s="21"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="16"/>
     </row>
     <row r="111" spans="6:7">
-      <c r="F111" s="21"/>
-      <c r="G111" s="21"/>
+      <c r="F111" s="16"/>
+      <c r="G111" s="16"/>
     </row>
     <row r="112" spans="6:7">
-      <c r="F112" s="21"/>
-      <c r="G112" s="21"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="16"/>
     </row>
     <row r="113" spans="6:7">
-      <c r="F113" s="21"/>
-      <c r="G113" s="21"/>
+      <c r="F113" s="16"/>
+      <c r="G113" s="16"/>
     </row>
     <row r="114" spans="6:7">
-      <c r="F114" s="21"/>
-      <c r="G114" s="21"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="16"/>
     </row>
     <row r="115" spans="6:7">
-      <c r="F115" s="21"/>
-      <c r="G115" s="21"/>
+      <c r="F115" s="16"/>
+      <c r="G115" s="16"/>
     </row>
     <row r="116" spans="6:7">
-      <c r="F116" s="21"/>
-      <c r="G116" s="21"/>
+      <c r="F116" s="16"/>
+      <c r="G116" s="16"/>
     </row>
     <row r="117" spans="6:7">
-      <c r="F117" s="21"/>
-      <c r="G117" s="21"/>
+      <c r="F117" s="16"/>
+      <c r="G117" s="16"/>
     </row>
     <row r="118" spans="6:7">
-      <c r="F118" s="21"/>
-      <c r="G118" s="21"/>
+      <c r="F118" s="16"/>
+      <c r="G118" s="16"/>
     </row>
     <row r="119" spans="6:7">
-      <c r="F119" s="21"/>
-      <c r="G119" s="21"/>
+      <c r="F119" s="16"/>
+      <c r="G119" s="16"/>
     </row>
     <row r="120" spans="6:7">
-      <c r="F120" s="21"/>
-      <c r="G120" s="21"/>
+      <c r="F120" s="16"/>
+      <c r="G120" s="16"/>
     </row>
     <row r="121" spans="6:7">
-      <c r="F121" s="21"/>
-      <c r="G121" s="21"/>
+      <c r="F121" s="16"/>
+      <c r="G121" s="16"/>
     </row>
     <row r="122" spans="6:7">
-      <c r="F122" s="21"/>
-      <c r="G122" s="21"/>
+      <c r="F122" s="16"/>
+      <c r="G122" s="16"/>
     </row>
     <row r="123" spans="6:7">
-      <c r="F123" s="21"/>
-      <c r="G123" s="21"/>
+      <c r="F123" s="16"/>
+      <c r="G123" s="16"/>
     </row>
     <row r="124" spans="6:7">
-      <c r="F124" s="21"/>
-      <c r="G124" s="21"/>
+      <c r="F124" s="16"/>
+      <c r="G124" s="16"/>
     </row>
     <row r="125" spans="6:7">
-      <c r="F125" s="21"/>
-      <c r="G125" s="21"/>
+      <c r="F125" s="16"/>
+      <c r="G125" s="16"/>
     </row>
     <row r="126" spans="6:7">
-      <c r="F126" s="21"/>
-      <c r="G126" s="21"/>
+      <c r="F126" s="16"/>
+      <c r="G126" s="16"/>
     </row>
     <row r="127" spans="6:7">
-      <c r="F127" s="21"/>
-      <c r="G127" s="21"/>
+      <c r="F127" s="16"/>
+      <c r="G127" s="16"/>
     </row>
     <row r="128" spans="6:7">
-      <c r="F128" s="21"/>
-      <c r="G128" s="21"/>
+      <c r="F128" s="16"/>
+      <c r="G128" s="16"/>
     </row>
     <row r="129" spans="6:7">
-      <c r="F129" s="21"/>
-      <c r="G129" s="21"/>
+      <c r="F129" s="16"/>
+      <c r="G129" s="16"/>
     </row>
     <row r="130" spans="6:7">
-      <c r="F130" s="21"/>
-      <c r="G130" s="21"/>
+      <c r="F130" s="16"/>
+      <c r="G130" s="16"/>
     </row>
     <row r="131" spans="6:7">
-      <c r="F131" s="21"/>
-      <c r="G131" s="21"/>
+      <c r="F131" s="16"/>
+      <c r="G131" s="16"/>
     </row>
     <row r="132" spans="6:7">
-      <c r="F132" s="21"/>
-      <c r="G132" s="21"/>
+      <c r="F132" s="16"/>
+      <c r="G132" s="16"/>
     </row>
     <row r="133" spans="6:7">
-      <c r="F133" s="21"/>
-      <c r="G133" s="21"/>
+      <c r="F133" s="16"/>
+      <c r="G133" s="16"/>
     </row>
     <row r="134" spans="6:7">
-      <c r="F134" s="21"/>
-      <c r="G134" s="21"/>
+      <c r="F134" s="16"/>
+      <c r="G134" s="16"/>
     </row>
     <row r="135" spans="6:7">
-      <c r="F135" s="21"/>
-      <c r="G135" s="21"/>
+      <c r="F135" s="16"/>
+      <c r="G135" s="16"/>
     </row>
     <row r="136" spans="6:7">
-      <c r="F136" s="21"/>
-      <c r="G136" s="21"/>
+      <c r="F136" s="16"/>
+      <c r="G136" s="16"/>
     </row>
     <row r="137" spans="6:7">
-      <c r="F137" s="21"/>
-      <c r="G137" s="21"/>
+      <c r="F137" s="16"/>
+      <c r="G137" s="16"/>
     </row>
     <row r="138" spans="6:7">
-      <c r="F138" s="21"/>
-      <c r="G138" s="21"/>
+      <c r="F138" s="16"/>
+      <c r="G138" s="16"/>
     </row>
     <row r="139" spans="6:7">
-      <c r="F139" s="21"/>
-      <c r="G139" s="21"/>
+      <c r="F139" s="16"/>
+      <c r="G139" s="16"/>
     </row>
     <row r="140" spans="6:7">
-      <c r="F140" s="21"/>
-      <c r="G140" s="21"/>
+      <c r="F140" s="16"/>
+      <c r="G140" s="16"/>
     </row>
     <row r="141" spans="6:7">
-      <c r="F141" s="21"/>
-      <c r="G141" s="21"/>
+      <c r="F141" s="16"/>
+      <c r="G141" s="16"/>
     </row>
     <row r="142" spans="6:7">
-      <c r="F142" s="21"/>
-      <c r="G142" s="21"/>
+      <c r="F142" s="16"/>
+      <c r="G142" s="16"/>
     </row>
     <row r="143" spans="6:7">
-      <c r="F143" s="21"/>
-      <c r="G143" s="21"/>
+      <c r="F143" s="16"/>
+      <c r="G143" s="16"/>
     </row>
     <row r="144" spans="6:7">
-      <c r="F144" s="21"/>
-      <c r="G144" s="21"/>
+      <c r="F144" s="16"/>
+      <c r="G144" s="16"/>
     </row>
     <row r="145" spans="6:7">
-      <c r="F145" s="21"/>
-      <c r="G145" s="21"/>
+      <c r="F145" s="16"/>
+      <c r="G145" s="16"/>
     </row>
     <row r="146" spans="6:7">
-      <c r="F146" s="21"/>
-      <c r="G146" s="21"/>
+      <c r="F146" s="16"/>
+      <c r="G146" s="16"/>
     </row>
     <row r="147" spans="6:7">
-      <c r="F147" s="21"/>
-      <c r="G147" s="21"/>
+      <c r="F147" s="16"/>
+      <c r="G147" s="16"/>
     </row>
     <row r="148" spans="6:7">
-      <c r="F148" s="21"/>
-      <c r="G148" s="21"/>
+      <c r="F148" s="16"/>
+      <c r="G148" s="16"/>
     </row>
     <row r="149" spans="6:7">
-      <c r="F149" s="21"/>
-      <c r="G149" s="21"/>
+      <c r="F149" s="16"/>
+      <c r="G149" s="16"/>
     </row>
     <row r="150" spans="6:7">
-      <c r="F150" s="21"/>
-      <c r="G150" s="21"/>
+      <c r="F150" s="16"/>
+      <c r="G150" s="16"/>
     </row>
     <row r="151" spans="6:7">
-      <c r="F151" s="21"/>
-      <c r="G151" s="21"/>
+      <c r="F151" s="16"/>
+      <c r="G151" s="16"/>
     </row>
     <row r="152" spans="6:7">
-      <c r="F152" s="21"/>
-      <c r="G152" s="21"/>
+      <c r="F152" s="16"/>
+      <c r="G152" s="16"/>
     </row>
     <row r="153" spans="6:7">
-      <c r="F153" s="21"/>
-      <c r="G153" s="21"/>
+      <c r="F153" s="16"/>
+      <c r="G153" s="16"/>
     </row>
     <row r="154" spans="6:7">
-      <c r="F154" s="21"/>
-      <c r="G154" s="21"/>
+      <c r="F154" s="16"/>
+      <c r="G154" s="16"/>
     </row>
     <row r="155" spans="6:7">
-      <c r="F155" s="21"/>
-      <c r="G155" s="21"/>
+      <c r="F155" s="16"/>
+      <c r="G155" s="16"/>
     </row>
     <row r="156" spans="6:7">
-      <c r="F156" s="21"/>
-      <c r="G156" s="21"/>
+      <c r="F156" s="16"/>
+      <c r="G156" s="16"/>
     </row>
     <row r="157" spans="6:7">
-      <c r="F157" s="21"/>
-      <c r="G157" s="21"/>
+      <c r="F157" s="16"/>
+      <c r="G157" s="16"/>
     </row>
     <row r="158" spans="6:7">
-      <c r="F158" s="21"/>
-      <c r="G158" s="21"/>
+      <c r="F158" s="16"/>
+      <c r="G158" s="16"/>
     </row>
     <row r="159" spans="6:7">
-      <c r="F159" s="21"/>
-      <c r="G159" s="21"/>
+      <c r="F159" s="16"/>
+      <c r="G159" s="16"/>
     </row>
     <row r="160" spans="6:7">
-      <c r="F160" s="21"/>
-      <c r="G160" s="21"/>
+      <c r="F160" s="16"/>
+      <c r="G160" s="16"/>
     </row>
     <row r="161" spans="6:7">
-      <c r="F161" s="21"/>
-      <c r="G161" s="21"/>
+      <c r="F161" s="16"/>
+      <c r="G161" s="16"/>
     </row>
     <row r="162" spans="6:7">
-      <c r="F162" s="21"/>
-      <c r="G162" s="21"/>
+      <c r="F162" s="16"/>
+      <c r="G162" s="16"/>
     </row>
     <row r="163" spans="6:7">
-      <c r="F163" s="21"/>
-      <c r="G163" s="21"/>
+      <c r="F163" s="16"/>
+      <c r="G163" s="16"/>
     </row>
     <row r="164" spans="6:7">
-      <c r="F164" s="21"/>
-      <c r="G164" s="21"/>
+      <c r="F164" s="16"/>
+      <c r="G164" s="16"/>
     </row>
     <row r="165" spans="6:7">
-      <c r="F165" s="21"/>
-      <c r="G165" s="21"/>
+      <c r="F165" s="16"/>
+      <c r="G165" s="16"/>
     </row>
     <row r="166" spans="6:7">
-      <c r="F166" s="21"/>
-      <c r="G166" s="21"/>
+      <c r="F166" s="16"/>
+      <c r="G166" s="16"/>
     </row>
     <row r="167" spans="6:7">
-      <c r="F167" s="21"/>
-      <c r="G167" s="21"/>
+      <c r="F167" s="16"/>
+      <c r="G167" s="16"/>
     </row>
     <row r="168" spans="6:7">
-      <c r="F168" s="21"/>
-      <c r="G168" s="21"/>
+      <c r="F168" s="16"/>
+      <c r="G168" s="16"/>
     </row>
     <row r="169" spans="6:7">
-      <c r="F169" s="21"/>
-      <c r="G169" s="21"/>
+      <c r="F169" s="16"/>
+      <c r="G169" s="16"/>
     </row>
     <row r="170" spans="6:7">
-      <c r="F170" s="21"/>
-      <c r="G170" s="21"/>
+      <c r="F170" s="16"/>
+      <c r="G170" s="16"/>
     </row>
     <row r="171" spans="6:7">
-      <c r="F171" s="21"/>
-      <c r="G171" s="21"/>
+      <c r="F171" s="16"/>
+      <c r="G171" s="16"/>
     </row>
     <row r="172" spans="6:7">
-      <c r="F172" s="21"/>
-      <c r="G172" s="21"/>
+      <c r="F172" s="16"/>
+      <c r="G172" s="16"/>
     </row>
     <row r="173" spans="6:7">
-      <c r="F173" s="21"/>
-      <c r="G173" s="21"/>
+      <c r="F173" s="16"/>
+      <c r="G173" s="16"/>
     </row>
     <row r="174" spans="6:7">
-      <c r="F174" s="21"/>
-      <c r="G174" s="21"/>
+      <c r="F174" s="16"/>
+      <c r="G174" s="16"/>
     </row>
     <row r="175" spans="6:7">
-      <c r="F175" s="21"/>
-      <c r="G175" s="21"/>
+      <c r="F175" s="16"/>
+      <c r="G175" s="16"/>
     </row>
     <row r="176" spans="6:7">
-      <c r="F176" s="21"/>
-      <c r="G176" s="21"/>
+      <c r="F176" s="16"/>
+      <c r="G176" s="16"/>
     </row>
     <row r="177" spans="6:7">
-      <c r="F177" s="21"/>
-      <c r="G177" s="21"/>
+      <c r="F177" s="16"/>
+      <c r="G177" s="16"/>
     </row>
     <row r="178" spans="6:7">
-      <c r="F178" s="21"/>
-      <c r="G178" s="21"/>
+      <c r="F178" s="16"/>
+      <c r="G178" s="16"/>
     </row>
     <row r="179" spans="6:7">
-      <c r="F179" s="21"/>
-      <c r="G179" s="21"/>
+      <c r="F179" s="16"/>
+      <c r="G179" s="16"/>
     </row>
     <row r="180" spans="6:7">
-      <c r="F180" s="21"/>
-      <c r="G180" s="21"/>
+      <c r="F180" s="16"/>
+      <c r="G180" s="16"/>
     </row>
     <row r="181" spans="6:7">
-      <c r="F181" s="21"/>
-      <c r="G181" s="21"/>
+      <c r="F181" s="16"/>
+      <c r="G181" s="16"/>
     </row>
     <row r="182" spans="6:7">
-      <c r="F182" s="21"/>
-      <c r="G182" s="21"/>
+      <c r="F182" s="16"/>
+      <c r="G182" s="16"/>
     </row>
     <row r="183" spans="6:7">
-      <c r="F183" s="21"/>
-      <c r="G183" s="21"/>
+      <c r="F183" s="16"/>
+      <c r="G183" s="16"/>
     </row>
     <row r="184" spans="6:7">
-      <c r="F184" s="21"/>
-      <c r="G184" s="21"/>
+      <c r="F184" s="16"/>
+      <c r="G184" s="16"/>
     </row>
     <row r="185" spans="6:7">
-      <c r="F185" s="21"/>
-      <c r="G185" s="21"/>
+      <c r="F185" s="16"/>
+      <c r="G185" s="16"/>
     </row>
     <row r="186" spans="6:7">
-      <c r="F186" s="21"/>
-      <c r="G186" s="21"/>
+      <c r="F186" s="16"/>
+      <c r="G186" s="16"/>
     </row>
     <row r="187" spans="6:7">
-      <c r="F187" s="21"/>
-      <c r="G187" s="21"/>
+      <c r="F187" s="16"/>
+      <c r="G187" s="16"/>
     </row>
     <row r="188" spans="6:7">
-      <c r="F188" s="21"/>
-      <c r="G188" s="21"/>
+      <c r="F188" s="16"/>
+      <c r="G188" s="16"/>
     </row>
     <row r="189" spans="6:7">
-      <c r="F189" s="21"/>
-      <c r="G189" s="21"/>
+      <c r="F189" s="16"/>
+      <c r="G189" s="16"/>
     </row>
     <row r="190" spans="6:7">
-      <c r="F190" s="21"/>
-      <c r="G190" s="21"/>
+      <c r="F190" s="16"/>
+      <c r="G190" s="16"/>
     </row>
     <row r="191" spans="6:7">
-      <c r="F191" s="21"/>
-      <c r="G191" s="21"/>
+      <c r="F191" s="16"/>
+      <c r="G191" s="16"/>
     </row>
     <row r="192" spans="6:7">
-      <c r="F192" s="21"/>
-      <c r="G192" s="21"/>
+      <c r="F192" s="16"/>
+      <c r="G192" s="16"/>
     </row>
     <row r="193" spans="6:7">
-      <c r="F193" s="21"/>
-      <c r="G193" s="21"/>
+      <c r="F193" s="16"/>
+      <c r="G193" s="16"/>
     </row>
     <row r="194" spans="6:7">
-      <c r="F194" s="21"/>
-      <c r="G194" s="21"/>
+      <c r="F194" s="16"/>
+      <c r="G194" s="16"/>
     </row>
     <row r="195" spans="6:7">
-      <c r="F195" s="21"/>
-      <c r="G195" s="21"/>
+      <c r="F195" s="16"/>
+      <c r="G195" s="16"/>
     </row>
     <row r="196" spans="6:7">
-      <c r="F196" s="21"/>
-      <c r="G196" s="21"/>
+      <c r="F196" s="16"/>
+      <c r="G196" s="16"/>
     </row>
     <row r="197" spans="6:7">
-      <c r="F197" s="21"/>
-      <c r="G197" s="21"/>
+      <c r="F197" s="16"/>
+      <c r="G197" s="16"/>
     </row>
     <row r="198" spans="6:7">
-      <c r="F198" s="21"/>
-      <c r="G198" s="21"/>
+      <c r="F198" s="16"/>
+      <c r="G198" s="16"/>
     </row>
     <row r="199" spans="6:7">
-      <c r="F199" s="21"/>
-      <c r="G199" s="21"/>
+      <c r="F199" s="16"/>
+      <c r="G199" s="16"/>
     </row>
     <row r="200" spans="6:7">
-      <c r="F200" s="21"/>
-      <c r="G200" s="21"/>
+      <c r="F200" s="16"/>
+      <c r="G200" s="16"/>
     </row>
     <row r="201" spans="6:7">
-      <c r="F201" s="21"/>
-      <c r="G201" s="21"/>
+      <c r="F201" s="16"/>
+      <c r="G201" s="16"/>
     </row>
     <row r="202" spans="6:7">
-      <c r="F202" s="21"/>
-      <c r="G202" s="21"/>
+      <c r="F202" s="16"/>
+      <c r="G202" s="16"/>
     </row>
     <row r="203" spans="6:7">
-      <c r="F203" s="21"/>
-      <c r="G203" s="21"/>
+      <c r="F203" s="16"/>
+      <c r="G203" s="16"/>
     </row>
     <row r="204" spans="6:7">
-      <c r="F204" s="21"/>
-      <c r="G204" s="21"/>
+      <c r="F204" s="16"/>
+      <c r="G204" s="16"/>
     </row>
     <row r="205" spans="6:7">
-      <c r="F205" s="21"/>
-      <c r="G205" s="21"/>
+      <c r="F205" s="16"/>
+      <c r="G205" s="16"/>
     </row>
     <row r="206" spans="6:7">
-      <c r="F206" s="21"/>
-      <c r="G206" s="21"/>
+      <c r="F206" s="16"/>
+      <c r="G206" s="16"/>
     </row>
     <row r="207" spans="6:7">
-      <c r="F207" s="21"/>
-      <c r="G207" s="21"/>
+      <c r="F207" s="16"/>
+      <c r="G207" s="16"/>
     </row>
     <row r="208" spans="6:7">
-      <c r="F208" s="21"/>
-      <c r="G208" s="21"/>
+      <c r="F208" s="16"/>
+      <c r="G208" s="16"/>
     </row>
     <row r="209" spans="6:7">
-      <c r="F209" s="21"/>
-      <c r="G209" s="21"/>
+      <c r="F209" s="16"/>
+      <c r="G209" s="16"/>
     </row>
     <row r="210" spans="6:7">
-      <c r="F210" s="21"/>
-      <c r="G210" s="21"/>
+      <c r="F210" s="16"/>
+      <c r="G210" s="16"/>
     </row>
     <row r="211" spans="6:7">
-      <c r="F211" s="21"/>
-      <c r="G211" s="21"/>
+      <c r="F211" s="16"/>
+      <c r="G211" s="16"/>
     </row>
     <row r="212" spans="6:7">
-      <c r="F212" s="21"/>
-      <c r="G212" s="21"/>
+      <c r="F212" s="16"/>
+      <c r="G212" s="16"/>
     </row>
     <row r="213" spans="6:7">
-      <c r="F213" s="21"/>
-      <c r="G213" s="21"/>
+      <c r="F213" s="16"/>
+      <c r="G213" s="16"/>
     </row>
     <row r="214" spans="6:7">
-      <c r="F214" s="21"/>
-      <c r="G214" s="21"/>
+      <c r="F214" s="16"/>
+      <c r="G214" s="16"/>
     </row>
     <row r="215" spans="6:7">
-      <c r="F215" s="21"/>
-      <c r="G215" s="21"/>
+      <c r="F215" s="16"/>
+      <c r="G215" s="16"/>
     </row>
     <row r="216" spans="6:7">
-      <c r="F216" s="21"/>
-      <c r="G216" s="21"/>
+      <c r="F216" s="16"/>
+      <c r="G216" s="16"/>
     </row>
     <row r="217" spans="6:7">
-      <c r="F217" s="21"/>
-      <c r="G217" s="21"/>
+      <c r="F217" s="16"/>
+      <c r="G217" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
@@ -2788,31 +2824,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="42"/>
-    <col min="2" max="2" width="96.83203125" style="40" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="37"/>
+    <col min="2" max="2" width="96.83203125" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="38" customFormat="1">
-      <c r="A1" s="41"/>
-      <c r="B1" s="39" t="s">
+    <row r="1" spans="1:3" s="33" customFormat="1">
+      <c r="A1" s="36"/>
+      <c r="B1" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="33" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C2" t="s">
@@ -2820,10 +2856,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="35" t="s">
         <v>73</v>
       </c>
       <c r="C3" t="s">
@@ -2831,10 +2867,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="35" t="s">
         <v>76</v>
       </c>
       <c r="C4" t="s">
@@ -2842,28 +2878,28 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="45">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="35" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="35" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="57" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="35" t="s">
         <v>115</v>
       </c>
       <c r="C10" t="s">
@@ -2871,7 +2907,7 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C11" t="s">
@@ -2879,7 +2915,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="35" t="s">
         <v>116</v>
       </c>
       <c r="C12" t="s">
@@ -2887,7 +2923,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="35" t="s">
         <v>117</v>
       </c>
       <c r="C13" t="s">
@@ -2895,18 +2931,18 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="65" t="s">
+      <c r="C14" s="60" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="C15" s="60" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2931,25 +2967,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="76.33203125" style="56" customWidth="1"/>
+    <col min="1" max="1" width="76.33203125" style="51" customWidth="1"/>
     <col min="2" max="2" width="104.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="53" customFormat="1">
-      <c r="A2" s="54" t="s">
+    <row r="2" spans="1:2" s="48" customFormat="1">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="48" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="50" t="s">
         <v>96</v>
       </c>
       <c r="B3" t="s">
@@ -2957,7 +2993,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="51" t="s">
         <v>97</v>
       </c>
       <c r="B4" t="s">
@@ -2965,7 +3001,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="51" t="s">
         <v>99</v>
       </c>
       <c r="B5" t="s">
@@ -2973,7 +3009,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="30">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="51" t="s">
         <v>101</v>
       </c>
       <c r="B6" t="s">
@@ -2981,52 +3017,52 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="52" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="51" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="51" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="51" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="51" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="51" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="51" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="51" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="51" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="51" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>